<commit_message>
backend update 27th dec
</commit_message>
<xml_diff>
--- a/backend/uploads/currentinventory_3_uk_december2025.xlsx
+++ b/backend/uploads/currentinventory_3_uk_december2025.xlsx
@@ -636,16 +636,16 @@
         <v>488.58</v>
       </c>
       <c r="R2">
-        <v>5112</v>
+        <v>5124</v>
       </c>
       <c r="S2">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="T2">
         <v>0</v>
       </c>
       <c r="U2">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="V2">
         <v>4698</v>
@@ -689,10 +689,10 @@
         <v>64.69</v>
       </c>
       <c r="R3">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="S3">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="T3">
         <v>0</v>
@@ -742,16 +742,16 @@
         <v>31.9</v>
       </c>
       <c r="R4">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="S4">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="T4">
         <v>0</v>
       </c>
       <c r="U4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V4">
         <v>239</v>
@@ -848,10 +848,10 @@
         <v>34.69</v>
       </c>
       <c r="R6">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="S6">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="T6">
         <v>0</v>
@@ -901,10 +901,10 @@
         <v>100.55</v>
       </c>
       <c r="R7">
-        <v>934</v>
+        <v>936</v>
       </c>
       <c r="S7">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="T7">
         <v>0</v>
@@ -1092,16 +1092,16 @@
         <v>80.89</v>
       </c>
       <c r="R11">
-        <v>1165</v>
+        <v>1168</v>
       </c>
       <c r="S11">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="T11">
         <v>0</v>
       </c>
       <c r="U11">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="V11">
         <v>1064</v>
@@ -1330,16 +1330,16 @@
         <v>1091.13</v>
       </c>
       <c r="R16">
-        <v>10873</v>
+        <v>10895</v>
       </c>
       <c r="S16">
-        <v>933</v>
+        <v>942</v>
       </c>
       <c r="T16">
         <v>0</v>
       </c>
       <c r="U16">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="V16">
         <v>10026</v>

</xml_diff>

<commit_message>
frontend update code 27th
</commit_message>
<xml_diff>
--- a/backend/uploads/currentinventory_3_uk_december2025.xlsx
+++ b/backend/uploads/currentinventory_3_uk_december2025.xlsx
@@ -636,10 +636,10 @@
         <v>488.58</v>
       </c>
       <c r="R2">
-        <v>5124</v>
+        <v>5138</v>
       </c>
       <c r="S2">
-        <v>458</v>
+        <v>472</v>
       </c>
       <c r="T2">
         <v>0</v>
@@ -689,10 +689,10 @@
         <v>64.69</v>
       </c>
       <c r="R3">
-        <v>903</v>
+        <v>905</v>
       </c>
       <c r="S3">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="T3">
         <v>0</v>
@@ -742,10 +742,10 @@
         <v>31.9</v>
       </c>
       <c r="R4">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="S4">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="T4">
         <v>0</v>
@@ -901,10 +901,10 @@
         <v>100.55</v>
       </c>
       <c r="R7">
-        <v>936</v>
+        <v>944</v>
       </c>
       <c r="S7">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="T7">
         <v>0</v>
@@ -1039,10 +1039,10 @@
         <v>117.58</v>
       </c>
       <c r="R10">
-        <v>1019</v>
+        <v>1023</v>
       </c>
       <c r="S10">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="T10">
         <v>0</v>
@@ -1092,10 +1092,10 @@
         <v>80.89</v>
       </c>
       <c r="R11">
-        <v>1168</v>
+        <v>1172</v>
       </c>
       <c r="S11">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="T11">
         <v>0</v>
@@ -1330,10 +1330,10 @@
         <v>1091.13</v>
       </c>
       <c r="R16">
-        <v>10895</v>
+        <v>10928</v>
       </c>
       <c r="S16">
-        <v>942</v>
+        <v>975</v>
       </c>
       <c r="T16">
         <v>0</v>

</xml_diff>